<commit_message>
Nové 3D modely a testovací programy na základní desku.
</commit_message>
<xml_diff>
--- a/Cena a součástky.xlsx
+++ b/Cena a součástky.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
   <si>
     <t>Množství</t>
   </si>
@@ -114,9 +114,6 @@
     <t>DS18B20</t>
   </si>
   <si>
-    <t>MSS1038-702NLC 6.8uH</t>
-  </si>
-  <si>
     <t>Encoder motor</t>
   </si>
   <si>
@@ -286,6 +283,18 @@
   </si>
   <si>
     <t>LiPo-Aku Graupner 2/1100 7,4V s TAM konektorem</t>
+  </si>
+  <si>
+    <t>Už mám</t>
+  </si>
+  <si>
+    <t>Dokoupit</t>
+  </si>
+  <si>
+    <t>Dutinka na motory</t>
+  </si>
+  <si>
+    <t>MSS1038-702NLC 10uH</t>
   </si>
 </sst>
 </file>
@@ -300,7 +309,7 @@
     <numFmt numFmtId="167" formatCode="_-* #,##0.0\ &quot;Kč&quot;_-;\-* #,##0.0\ &quot;Kč&quot;_-;_-* &quot;-&quot;?\ &quot;Kč&quot;_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;Kč&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,8 +367,15 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,12 +408,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -405,12 +415,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -443,14 +447,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -464,7 +467,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -475,9 +477,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -816,7 +819,7 @@
       <c r="J5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="11" t="e">
+      <c r="K5" s="10" t="e">
         <f>I5/I6</f>
         <v>#DIV/0!</v>
       </c>
@@ -826,9 +829,9 @@
         <v>13</v>
       </c>
       <c r="D6" s="3"/>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <f>PlanSoucastekNaRobota!F4*E5</f>
-        <v>16182.870000000003</v>
+        <v>16214.79</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>15</v>
@@ -847,7 +850,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <f>15000-I6</f>
         <v>15000</v>
       </c>
@@ -878,83 +881,83 @@
       </c>
     </row>
     <row r="10" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C10" s="7"/>
-      <c r="I10" s="9"/>
+      <c r="C10" s="6"/>
+      <c r="I10" s="8"/>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I11" s="10"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I12" s="10"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I13" s="10"/>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I14" s="10"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I15" s="10"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I16" s="10"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I17" s="10"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I18" s="10"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I19" s="10"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I20" s="10"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I21" s="10"/>
+      <c r="I21" s="9"/>
     </row>
     <row r="22" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I22" s="10"/>
+      <c r="I22" s="9"/>
     </row>
     <row r="23" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I23" s="10"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I24" s="10"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I25" s="10"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="26" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I26" s="10"/>
+      <c r="I26" s="9"/>
     </row>
     <row r="27" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I27" s="10"/>
+      <c r="I27" s="9"/>
     </row>
     <row r="28" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I28" s="10"/>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I29" s="10"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I30" s="10"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I31" s="10"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I32" s="10"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I33" s="10"/>
+      <c r="I33" s="9"/>
     </row>
     <row r="34" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I34" s="10"/>
+      <c r="I34" s="9"/>
     </row>
     <row r="35" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I35" s="10"/>
+      <c r="I35" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I10:I52">
@@ -976,7 +979,7 @@
   <dimension ref="A2:Y48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X22" sqref="X22"/>
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,10 +987,10 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -997,7 +1000,7 @@
   <sheetData>
     <row r="2" spans="1:25" ht="31.5" x14ac:dyDescent="0.5">
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
@@ -1008,10 +1011,10 @@
       <c r="E4" s="3"/>
       <c r="F4" s="5">
         <f>SUM(R13:R50)</f>
-        <v>1618.2870000000003</v>
+        <v>1621.479</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3">
@@ -1020,37 +1023,37 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="I5" t="s">
-        <v>64</v>
-      </c>
-      <c r="K5" s="23">
+        <v>63</v>
+      </c>
+      <c r="K5" s="21">
         <v>21.48</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C6" s="14"/>
+      <c r="C6" s="13"/>
       <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="15"/>
+      <c r="F6" s="14"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C7" s="12"/>
+      <c r="C7" s="11"/>
       <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="C8" s="17"/>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="C9" s="23"/>
+      <c r="D9" t="s">
         <v>82</v>
-      </c>
-      <c r="F7" s="15"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C8" s="18"/>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C9" s="25"/>
-      <c r="D9" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
@@ -1068,13 +1071,17 @@
       <c r="I12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J12" s="2"/>
+      <c r="J12" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="K12" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L12" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="M12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1083,11 +1090,11 @@
       </c>
       <c r="Q12" s="1"/>
       <c r="R12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
@@ -1095,910 +1102,1181 @@
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="12"/>
       <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="I13">
+      <c r="E13" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="I13" s="30">
         <v>1</v>
       </c>
-      <c r="K13">
+      <c r="J13" s="30">
+        <v>5</v>
+      </c>
+      <c r="K13" s="30">
         <f>I13*($K$4)</f>
         <v>5</v>
       </c>
-      <c r="M13" s="19"/>
-      <c r="P13" s="21">
+      <c r="L13">
+        <f>K13-J13</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="18"/>
+      <c r="P13" s="19">
         <v>147</v>
       </c>
-      <c r="R13" s="22">
+      <c r="R13" s="20">
         <f t="shared" ref="R13:R44" si="0">P13*I13</f>
         <v>147</v>
       </c>
-      <c r="T13" s="22">
+      <c r="T13" s="20">
         <f>K13*P13</f>
         <v>735</v>
       </c>
-      <c r="W13" s="16"/>
-      <c r="Y13" s="24"/>
+      <c r="W13" s="15"/>
+      <c r="Y13" s="22"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
+      <c r="A14" s="28"/>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
-      </c>
-      <c r="I14">
+        <v>38</v>
+      </c>
+      <c r="I14" s="30">
         <v>1</v>
       </c>
-      <c r="K14">
-        <f t="shared" ref="K14:K44" si="1">I14*($K$4)</f>
-        <v>5</v>
-      </c>
-      <c r="M14" s="12"/>
-      <c r="P14" s="21">
+      <c r="J14" s="30">
+        <v>2</v>
+      </c>
+      <c r="K14" s="30">
+        <f t="shared" ref="K14:K42" si="1">I14*($K$4)</f>
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ref="L14:L44" si="2">K14-J14</f>
+        <v>3</v>
+      </c>
+      <c r="M14" s="11"/>
+      <c r="P14" s="19">
         <v>6</v>
       </c>
-      <c r="R14" s="22">
+      <c r="R14" s="20">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="T14" s="22">
-        <f t="shared" ref="T14:T44" si="2">K14*P14</f>
+      <c r="T14" s="20">
+        <f t="shared" ref="T14:T44" si="3">K14*P14</f>
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" t="s">
-        <v>53</v>
+      <c r="A15" s="11"/>
+      <c r="B15" s="12" t="s">
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15">
+        <v>89</v>
+      </c>
+      <c r="I15" s="30">
         <v>1</v>
       </c>
-      <c r="K15">
-        <v>5</v>
-      </c>
-      <c r="M15" s="13"/>
-      <c r="P15" s="21">
+      <c r="J15" s="30">
+        <v>2</v>
+      </c>
+      <c r="K15" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M15" s="12"/>
+      <c r="P15" s="19">
         <v>72</v>
       </c>
-      <c r="R15" s="22">
+      <c r="R15" s="20">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="T15" s="22">
-        <f t="shared" si="2"/>
+      <c r="T15" s="20">
+        <f t="shared" si="3"/>
         <v>360</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" t="s">
-        <v>51</v>
+      <c r="A16" s="11"/>
+      <c r="B16" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="E16" t="s">
+        <v>71</v>
+      </c>
+      <c r="I16" s="30">
+        <v>1</v>
+      </c>
+      <c r="J16" s="30">
+        <v>2</v>
+      </c>
+      <c r="K16" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M16" s="12"/>
+      <c r="P16" s="19">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="R16" s="20">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="T16" s="20">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="s">
         <v>72</v>
       </c>
-      <c r="I16">
+      <c r="I17" s="30">
         <v>1</v>
       </c>
-      <c r="K16">
-        <v>5</v>
-      </c>
-      <c r="M16" s="13"/>
-      <c r="P16" s="21">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="R16" s="22">
-        <f t="shared" si="0"/>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="T16" s="22">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" t="s">
-        <v>73</v>
-      </c>
-      <c r="I17">
+      <c r="J17" s="30">
+        <v>2</v>
+      </c>
+      <c r="K17" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M17" s="12"/>
+      <c r="P17" s="19">
+        <v>11.2</v>
+      </c>
+      <c r="R17" s="20">
+        <f t="shared" si="0"/>
+        <v>11.2</v>
+      </c>
+      <c r="T17" s="20">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I18" s="30">
         <v>1</v>
       </c>
-      <c r="K17">
-        <v>5</v>
-      </c>
-      <c r="M17" s="13"/>
-      <c r="P17" s="21">
-        <v>11.2</v>
-      </c>
-      <c r="R17" s="22">
-        <f t="shared" si="0"/>
-        <v>11.2</v>
-      </c>
-      <c r="T17" s="22">
-        <f t="shared" si="2"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M18" s="12"/>
-      <c r="P18" s="21">
+      <c r="J18" s="30">
+        <v>5</v>
+      </c>
+      <c r="K18" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="11"/>
+      <c r="P18" s="19">
         <v>138</v>
       </c>
-      <c r="R18" s="22">
+      <c r="R18" s="20">
         <f t="shared" si="0"/>
         <v>138</v>
       </c>
-      <c r="T18" s="22">
-        <f t="shared" si="2"/>
+      <c r="T18" s="20">
+        <f t="shared" si="3"/>
         <v>690</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
+      <c r="A19" s="26"/>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="30">
         <v>1</v>
       </c>
-      <c r="K19">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M19" s="18"/>
-      <c r="P19" s="21"/>
-      <c r="R19" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T19" s="22">
-        <f t="shared" si="2"/>
+      <c r="J19" s="30">
+        <v>0</v>
+      </c>
+      <c r="K19" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="M19" s="17"/>
+      <c r="P19" s="19"/>
+      <c r="R19" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T19" s="20">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
+      <c r="A20" s="12"/>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="20">
-        <v>2</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I20" s="30">
+        <v>2</v>
+      </c>
+      <c r="J20" s="30">
         <v>10</v>
       </c>
-      <c r="M20" s="30"/>
-      <c r="P20" s="21">
+      <c r="K20" s="30">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="27"/>
+      <c r="P20" s="19">
         <v>4</v>
       </c>
-      <c r="R20" s="22">
+      <c r="R20" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="T20" s="22">
-        <f t="shared" si="2"/>
+      <c r="T20" s="20">
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
+      <c r="A21" s="28"/>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>31</v>
-      </c>
-      <c r="I21">
+        <v>30</v>
+      </c>
+      <c r="I21" s="30">
         <v>1</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M21" s="12"/>
-      <c r="P21" s="21">
+      <c r="J21" s="30">
+        <v>3</v>
+      </c>
+      <c r="K21" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M21" s="11"/>
+      <c r="P21" s="19">
         <v>78</v>
       </c>
-      <c r="R21" s="22">
+      <c r="R21" s="20">
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="T21" s="22">
-        <f t="shared" si="2"/>
+      <c r="T21" s="20">
+        <f t="shared" si="3"/>
         <v>390</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
+      <c r="A22" s="11"/>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
         <v>26</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="30">
         <v>0.2</v>
       </c>
-      <c r="K22">
+      <c r="J22" s="30">
+        <v>0</v>
+      </c>
+      <c r="K22" s="30">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M22" s="18"/>
-      <c r="P22" s="21">
+      <c r="L22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M22" s="17"/>
+      <c r="P22" s="19">
         <f>40*K5</f>
         <v>859.2</v>
       </c>
-      <c r="R22" s="22">
+      <c r="R22" s="20">
         <f t="shared" si="0"/>
         <v>171.84000000000003</v>
       </c>
-      <c r="T22" s="22">
-        <f t="shared" si="2"/>
+      <c r="T22" s="20">
+        <f t="shared" si="3"/>
         <v>859.2</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="31"/>
+      <c r="A23" s="12"/>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
-      </c>
-      <c r="I23">
+        <v>33</v>
+      </c>
+      <c r="I23" s="30">
         <v>1</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M23" s="30"/>
-      <c r="P23" s="21">
+      <c r="J23" s="30">
+        <v>5</v>
+      </c>
+      <c r="K23" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="27"/>
+      <c r="P23" s="19">
         <v>3</v>
       </c>
-      <c r="R23" s="22">
+      <c r="R23" s="20">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="T23" s="22">
-        <f t="shared" si="2"/>
+      <c r="T23" s="20">
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="31"/>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
+      <c r="A24" s="11"/>
+      <c r="B24" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="12"/>
       <c r="E24" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="30">
+        <v>3</v>
+      </c>
+      <c r="J24" s="30">
+        <v>11</v>
+      </c>
+      <c r="K24" s="30">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="M24" s="12"/>
+      <c r="P24" s="19">
+        <v>6.1550000000000002</v>
+      </c>
+      <c r="R24" s="20">
+        <f t="shared" si="0"/>
+        <v>18.465</v>
+      </c>
+      <c r="T24" s="20">
+        <f t="shared" si="3"/>
+        <v>92.325000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="E25" t="s">
         <v>40</v>
       </c>
-      <c r="I24">
-        <v>3</v>
-      </c>
-      <c r="K24">
-        <v>20</v>
-      </c>
-      <c r="M24" s="13"/>
-      <c r="P24" s="21">
-        <v>6.1550000000000002</v>
-      </c>
-      <c r="R24" s="22">
-        <f t="shared" si="0"/>
-        <v>18.465</v>
-      </c>
-      <c r="T24" s="22">
-        <f t="shared" si="2"/>
-        <v>123.10000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="31"/>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" t="s">
-        <v>41</v>
-      </c>
-      <c r="I25">
+      <c r="I25" s="30">
         <v>1</v>
       </c>
-      <c r="K25">
+      <c r="J25" s="30">
+        <v>7</v>
+      </c>
+      <c r="K25" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="M25" s="12"/>
+      <c r="P25" s="19">
+        <v>1.52</v>
+      </c>
+      <c r="R25" s="20">
+        <f t="shared" si="0"/>
+        <v>1.52</v>
+      </c>
+      <c r="T25" s="20">
+        <f t="shared" si="3"/>
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" t="s">
+        <v>80</v>
+      </c>
+      <c r="I26" s="30">
+        <v>1</v>
+      </c>
+      <c r="J26" s="30">
+        <v>5</v>
+      </c>
+      <c r="K26" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="17"/>
+      <c r="P26" s="19">
+        <v>15</v>
+      </c>
+      <c r="R26" s="20">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="T26" s="20">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="28"/>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" s="30">
+        <v>2</v>
+      </c>
+      <c r="J27" s="30">
+        <v>8</v>
+      </c>
+      <c r="K27" s="30">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="M25" s="13"/>
-      <c r="P25" s="21">
-        <v>1.52</v>
-      </c>
-      <c r="R25" s="22">
-        <f t="shared" si="0"/>
-        <v>1.52</v>
-      </c>
-      <c r="T25" s="22">
-        <f t="shared" si="2"/>
-        <v>15.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" t="s">
-        <v>81</v>
-      </c>
-      <c r="I26" s="6">
-        <v>1</v>
-      </c>
-      <c r="K26">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M26" s="18"/>
-      <c r="P26" s="21">
-        <v>15</v>
-      </c>
-      <c r="R26" s="22">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="T26" s="22">
-        <f t="shared" si="2"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="31"/>
-      <c r="B27" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" t="s">
-        <v>69</v>
-      </c>
-      <c r="I27" s="6">
-        <v>2</v>
-      </c>
-      <c r="K27">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="M27" s="12"/>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M27" s="11"/>
       <c r="P27">
         <v>0.8</v>
       </c>
-      <c r="R27" s="22">
+      <c r="R27" s="20">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="T27" s="22">
-        <f t="shared" si="2"/>
+      <c r="T27" s="20">
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="32"/>
+      <c r="A28" s="12"/>
       <c r="B28" t="s">
         <v>24</v>
       </c>
       <c r="E28" t="s">
-        <v>63</v>
-      </c>
-      <c r="I28" s="6">
+        <v>62</v>
+      </c>
+      <c r="I28" s="30">
         <v>1</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M28" s="19"/>
-      <c r="P28" s="21"/>
-      <c r="R28" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T28" s="22">
-        <f t="shared" si="2"/>
+      <c r="J28" s="30">
+        <v>5</v>
+      </c>
+      <c r="K28" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="18"/>
+      <c r="P28" s="19"/>
+      <c r="R28" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T28" s="20">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="W28">
         <v>1200.52</v>
       </c>
       <c r="X28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
+      <c r="A29" s="12"/>
       <c r="B29" t="s">
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
-      </c>
-      <c r="I29">
+        <v>32</v>
+      </c>
+      <c r="I29" s="30">
         <v>1</v>
       </c>
-      <c r="K29">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M29" s="18"/>
-      <c r="P29" s="21"/>
-      <c r="R29" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T29" s="22">
-        <f t="shared" si="2"/>
+      <c r="J29" s="30">
+        <v>5</v>
+      </c>
+      <c r="K29" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="17"/>
+      <c r="P29" s="19"/>
+      <c r="R29" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="20">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="31"/>
+      <c r="A30" s="12"/>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E30" t="s">
-        <v>30</v>
-      </c>
-      <c r="I30">
-        <v>2</v>
-      </c>
-      <c r="K30">
-        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I30" s="30">
+        <v>2</v>
+      </c>
+      <c r="J30" s="30">
         <v>10</v>
       </c>
-      <c r="M30" s="26"/>
-      <c r="P30" s="21">
+      <c r="K30" s="30">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="24"/>
+      <c r="P30" s="19">
         <v>345</v>
       </c>
-      <c r="R30" s="22">
+      <c r="R30" s="20">
         <f t="shared" si="0"/>
         <v>690</v>
       </c>
-      <c r="T30" s="22">
-        <f t="shared" si="2"/>
+      <c r="T30" s="20">
+        <f t="shared" si="3"/>
         <v>3450</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
+      <c r="A31" s="12"/>
       <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" t="s">
         <v>70</v>
       </c>
-      <c r="E31" t="s">
-        <v>71</v>
-      </c>
-      <c r="I31" s="6">
-        <v>2</v>
-      </c>
-      <c r="K31">
-        <f t="shared" si="1"/>
+      <c r="I31" s="30">
+        <v>2</v>
+      </c>
+      <c r="J31" s="30">
         <v>10</v>
       </c>
-      <c r="M31" s="18"/>
-      <c r="R31" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T31" s="22">
-        <f t="shared" si="2"/>
+      <c r="K31" s="30">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M31" s="17"/>
+      <c r="R31" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T31" s="20">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" t="s">
-        <v>59</v>
-      </c>
+      <c r="A32" s="11"/>
+      <c r="B32" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="12"/>
       <c r="E32" t="s">
-        <v>32</v>
-      </c>
-      <c r="I32">
+        <v>31</v>
+      </c>
+      <c r="I32" s="30">
         <v>1</v>
       </c>
-      <c r="K32">
-        <v>5</v>
-      </c>
-      <c r="M32" s="13"/>
-      <c r="P32" s="21">
+      <c r="J32" s="30">
+        <v>2</v>
+      </c>
+      <c r="K32" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M32" s="12"/>
+      <c r="P32" s="19">
         <v>49</v>
       </c>
-      <c r="R32" s="22">
+      <c r="R32" s="20">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="T32" s="22">
-        <f t="shared" si="2"/>
+      <c r="T32" s="20">
+        <f t="shared" si="3"/>
         <v>245</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" t="s">
+      <c r="A33" s="11"/>
+      <c r="B33" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="30">
+        <v>2</v>
+      </c>
+      <c r="J33" s="30">
+        <v>6</v>
+      </c>
+      <c r="K33" s="30">
+        <f>I33*($K$4)</f>
+        <v>10</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="M33" s="12"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="19">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="R33" s="20">
+        <f t="shared" si="0"/>
+        <v>1.5580000000000001</v>
+      </c>
+      <c r="T33" s="20">
+        <f t="shared" si="3"/>
+        <v>7.79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" t="s">
+        <v>43</v>
+      </c>
+      <c r="I34" s="30">
+        <v>2</v>
+      </c>
+      <c r="J34" s="30">
+        <v>4</v>
+      </c>
+      <c r="K34" s="30">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M34" s="12"/>
+      <c r="P34" s="19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R34" s="20">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="T34" s="20">
+        <f t="shared" si="3"/>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
+      <c r="B35" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="I35" s="30">
+        <v>2</v>
+      </c>
+      <c r="J35" s="30">
+        <v>6</v>
+      </c>
+      <c r="K35" s="30">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="M35" s="12"/>
+      <c r="P35" s="19">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R35" s="20">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="T35" s="20">
+        <f t="shared" si="3"/>
+        <v>1.4000000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" t="s">
+        <v>45</v>
+      </c>
+      <c r="I36" s="30">
+        <v>5</v>
+      </c>
+      <c r="J36" s="30">
+        <v>6</v>
+      </c>
+      <c r="K36" s="30">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="M36" s="12"/>
+      <c r="P36" s="19">
+        <v>0.13</v>
+      </c>
+      <c r="R36" s="20">
+        <f t="shared" si="0"/>
+        <v>0.65</v>
+      </c>
+      <c r="T36" s="20">
+        <f t="shared" si="3"/>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
+      <c r="B37" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" s="30">
+        <v>2</v>
+      </c>
+      <c r="J37" s="30">
+        <v>8</v>
+      </c>
+      <c r="K37" s="30">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M37" s="12"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="19">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="R37" s="20">
+        <f t="shared" si="0"/>
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="T37" s="20">
+        <f t="shared" si="3"/>
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" t="s">
         <v>57</v>
       </c>
-      <c r="E33" t="s">
-        <v>43</v>
-      </c>
-      <c r="I33">
+      <c r="E38" t="s">
+        <v>46</v>
+      </c>
+      <c r="I38" s="30">
         <v>1</v>
       </c>
-      <c r="K33">
-        <v>10</v>
-      </c>
-      <c r="M33" s="13"/>
-      <c r="O33" s="17"/>
-      <c r="P33" s="21">
-        <v>0.77900000000000003</v>
-      </c>
-      <c r="R33" s="22">
-        <f t="shared" si="0"/>
-        <v>0.77900000000000003</v>
-      </c>
-      <c r="T33" s="22">
-        <f t="shared" si="2"/>
-        <v>7.79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A34" s="31"/>
-      <c r="B34" t="s">
-        <v>57</v>
-      </c>
-      <c r="E34" t="s">
-        <v>44</v>
-      </c>
-      <c r="I34">
-        <v>1</v>
-      </c>
-      <c r="K34">
-        <v>10</v>
-      </c>
-      <c r="M34" s="13"/>
-      <c r="P34" s="21">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="R34" s="22">
-        <f t="shared" si="0"/>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="T34" s="22">
-        <f t="shared" si="2"/>
-        <v>1.4000000000000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A35" s="31"/>
-      <c r="B35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E35" t="s">
-        <v>45</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-      <c r="K35">
-        <v>10</v>
-      </c>
-      <c r="M35" s="13"/>
-      <c r="P35" s="21">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="R35" s="22">
-        <f t="shared" si="0"/>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="T35" s="22">
-        <f t="shared" si="2"/>
-        <v>1.4000000000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="31"/>
-      <c r="B36" t="s">
-        <v>57</v>
-      </c>
-      <c r="E36" t="s">
-        <v>46</v>
-      </c>
-      <c r="I36">
-        <v>2</v>
-      </c>
-      <c r="K36">
-        <v>10</v>
-      </c>
-      <c r="M36" s="13"/>
-      <c r="P36" s="21">
-        <v>0.13</v>
-      </c>
-      <c r="R36" s="22">
-        <f t="shared" si="0"/>
-        <v>0.26</v>
-      </c>
-      <c r="T36" s="22">
-        <f t="shared" si="2"/>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="31"/>
-      <c r="B37" t="s">
-        <v>57</v>
-      </c>
-      <c r="E37" t="s">
-        <v>75</v>
-      </c>
-      <c r="I37">
-        <v>1</v>
-      </c>
-      <c r="K37">
-        <v>10</v>
-      </c>
-      <c r="M37" s="13"/>
-      <c r="O37" s="17"/>
-      <c r="P37" s="21">
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="R37" s="22">
-        <f t="shared" si="0"/>
-        <v>0.14299999999999999</v>
-      </c>
-      <c r="T37" s="22">
-        <f t="shared" si="2"/>
-        <v>1.43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A38" s="31"/>
-      <c r="B38" t="s">
-        <v>58</v>
-      </c>
-      <c r="E38" t="s">
-        <v>47</v>
-      </c>
-      <c r="I38">
-        <v>1</v>
-      </c>
-      <c r="K38">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M38" s="12"/>
-      <c r="P38" s="21">
+      <c r="J38" s="30">
+        <v>5</v>
+      </c>
+      <c r="K38" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M38" s="11"/>
+      <c r="P38" s="19">
         <v>64</v>
       </c>
-      <c r="R38" s="22">
+      <c r="R38" s="20">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="T38" s="22">
-        <f t="shared" si="2"/>
+      <c r="T38" s="20">
+        <f t="shared" si="3"/>
         <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A39" s="31"/>
+      <c r="A39" s="28"/>
       <c r="B39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E39" t="s">
         <v>28</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="30">
         <v>1</v>
       </c>
-      <c r="K39">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M39" s="12"/>
-      <c r="P39" s="21">
+      <c r="J39" s="30">
+        <v>3</v>
+      </c>
+      <c r="K39" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M39" s="11"/>
+      <c r="P39" s="19">
         <v>38</v>
       </c>
-      <c r="R39" s="22">
+      <c r="R39" s="20">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="T39" s="22">
-        <f t="shared" si="2"/>
+      <c r="T39" s="20">
+        <f t="shared" si="3"/>
         <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="31"/>
-      <c r="B40" t="s">
-        <v>56</v>
+      <c r="A40" s="11"/>
+      <c r="B40" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
-      </c>
-      <c r="I40">
+        <v>73</v>
+      </c>
+      <c r="I40" s="30">
         <v>1</v>
       </c>
-      <c r="K40">
-        <v>5</v>
-      </c>
-      <c r="M40" s="13"/>
-      <c r="P40" s="21">
+      <c r="J40" s="30">
+        <v>2</v>
+      </c>
+      <c r="K40" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M40" s="12"/>
+      <c r="P40" s="19">
         <v>17.8</v>
       </c>
-      <c r="R40" s="22">
+      <c r="R40" s="20">
         <f t="shared" si="0"/>
         <v>17.8</v>
       </c>
-      <c r="T40" s="22">
-        <f t="shared" si="2"/>
+      <c r="T40" s="20">
+        <f t="shared" si="3"/>
         <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="31"/>
+      <c r="A41" s="29"/>
       <c r="B41" t="s">
         <v>9</v>
       </c>
       <c r="E41" t="s">
         <v>25</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="30">
         <v>1</v>
       </c>
-      <c r="K41">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M41" s="12"/>
-      <c r="P41" s="21">
+      <c r="J41" s="30">
+        <v>2</v>
+      </c>
+      <c r="K41" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M41" s="11"/>
+      <c r="N41" s="17"/>
+      <c r="P41" s="19">
         <v>8</v>
       </c>
-      <c r="R41" s="22">
+      <c r="R41" s="20">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="T41" s="22">
-        <f t="shared" si="2"/>
+      <c r="T41" s="20">
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="31"/>
+      <c r="A42" s="12"/>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E42" t="s">
         <v>4</v>
       </c>
-      <c r="I42" s="6">
+      <c r="I42" s="30">
         <v>1</v>
       </c>
-      <c r="K42">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="M42" s="27"/>
-      <c r="P42" s="21"/>
-      <c r="R42" s="21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T42" s="22">
-        <f t="shared" si="2"/>
+      <c r="J42" s="30">
+        <v>5</v>
+      </c>
+      <c r="K42" s="30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="25"/>
+      <c r="P42" s="19"/>
+      <c r="R42" s="19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T42" s="20">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A43" s="31"/>
+      <c r="A43" s="12"/>
       <c r="B43" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="E43" s="24" t="s">
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="J43" s="30">
+        <v>2</v>
+      </c>
+      <c r="K43" s="30">
+        <f t="shared" ref="K14:K44" si="4">I43*($K$4)</f>
+        <v>2</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="17"/>
+      <c r="P43" s="19">
+        <v>147</v>
+      </c>
+      <c r="R43" s="19">
+        <f t="shared" si="0"/>
+        <v>58.800000000000004</v>
+      </c>
+      <c r="T43" s="20">
+        <f t="shared" si="3"/>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" t="s">
         <v>78</v>
       </c>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="6">
+      <c r="E44" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="30">
         <v>0.4</v>
       </c>
-      <c r="K43">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M43" s="18"/>
-      <c r="P43" s="21">
-        <v>147</v>
-      </c>
-      <c r="R43" s="21">
-        <f t="shared" si="0"/>
-        <v>58.800000000000004</v>
-      </c>
-      <c r="T43" s="22">
-        <f t="shared" si="2"/>
-        <v>294</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" t="s">
-        <v>79</v>
-      </c>
-      <c r="E44" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="K44">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="M44" s="18"/>
-      <c r="P44" s="21">
+      <c r="J44" s="30">
+        <v>2</v>
+      </c>
+      <c r="K44" s="30">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="17"/>
+      <c r="P44" s="19">
         <v>38</v>
       </c>
-      <c r="R44" s="21">
+      <c r="R44" s="19">
         <f t="shared" si="0"/>
         <v>15.200000000000001</v>
       </c>
-      <c r="T44" s="22">
-        <f t="shared" si="2"/>
+      <c r="T44" s="20">
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="P45" s="21"/>
-      <c r="R45" s="21"/>
+      <c r="A45" s="28"/>
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+      <c r="E45" t="s">
+        <v>68</v>
+      </c>
+      <c r="I45" s="30">
+        <v>2</v>
+      </c>
+      <c r="J45" s="30">
+        <v>5</v>
+      </c>
+      <c r="K45" s="30">
+        <f t="shared" ref="K45" si="5">I45*($K$4)</f>
+        <v>10</v>
+      </c>
+      <c r="L45">
+        <f t="shared" ref="L45" si="6">K45-J45</f>
+        <v>5</v>
+      </c>
+      <c r="M45" s="11"/>
+      <c r="P45">
+        <v>0.8</v>
+      </c>
+      <c r="R45" s="20">
+        <f t="shared" ref="R45" si="7">P45*I45</f>
+        <v>1.6</v>
+      </c>
+      <c r="T45" s="20">
+        <f t="shared" ref="T45" si="8">K45*P45</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="P46" s="21"/>
-      <c r="R46" s="21"/>
+      <c r="P46" s="19"/>
+      <c r="R46" s="19"/>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="P47" s="21"/>
-      <c r="R47" s="21"/>
+      <c r="P47" s="19"/>
+      <c r="R47" s="19"/>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="P48" s="21"/>
-      <c r="R48" s="21"/>
+      <c r="P48" s="19"/>
+      <c r="R48" s="19"/>
     </row>
   </sheetData>
   <sortState ref="B13:T42">

</xml_diff>